<commit_message>
OO-1209 adding context help for import
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti/questionimport/qti-import-metadata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31080" windowHeight="21780" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31240" windowHeight="28280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
     <t>FIB</t>
   </si>
   <si>
-    <t>Fragetpy: Fill in the blanks</t>
-  </si>
-  <si>
     <t>Englisch: Grundwortschatz: ban</t>
   </si>
   <si>
@@ -216,30 +213,6 @@
     <t>Editor Version</t>
   </si>
   <si>
-    <t>Nur in Fragenpool : Schlagworte</t>
-  </si>
-  <si>
-    <t>Nur in Fragenpool : Abdeckung</t>
-  </si>
-  <si>
-    <t>Nur in Fragenpool : Sprache</t>
-  </si>
-  <si>
-    <t>Nur in Fragenpool : Fachbereich</t>
-  </si>
-  <si>
-    <t>Nur in Fragenpool : Level</t>
-  </si>
-  <si>
-    <t>Nur in Fragenpool : Editor Version</t>
-  </si>
-  <si>
-    <t>Nur in Fragenpool : probiert ein Lizenz mit dem gleichen Key zu finden oder erstellt eine neue Freitext Lizenz</t>
-  </si>
-  <si>
-    <t>Nur in Fragenpool : Durchschnittliche Bearbeitungszeit, Format ist unter http://www.w3.org/TR/xmlschema-2/#duration definiert</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -270,21 +243,6 @@
     <t>Primarschule</t>
   </si>
   <si>
-    <t>Nur in Fragenpool : Itemschwierigkeit (zwischen 0.0 und 1.0)</t>
-  </si>
-  <si>
-    <t>Nur in Fragenpool : Standardabweichung Itemschwierigkeit (zwischen 0.0 und 1.0)</t>
-  </si>
-  <si>
-    <t>Nur in Fragenpool : Trennschärfe (zwischen -1.0 und 1.0)</t>
-  </si>
-  <si>
-    <t>Nur in Fragenpool : Anzahl Distraktoren ( 1 )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nur in Fragenpool : Editor </t>
-  </si>
-  <si>
     <t>Question</t>
   </si>
   <si>
@@ -292,6 +250,48 @@
   </si>
   <si>
     <t>9.4.2</t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : Schlagworte</t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : Abdeckung</t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : Sprache</t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : Fachbereich</t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : probiert ein Lizenz mit dem gleichen Key zu finden oder erstellt eine neue Freitext Lizenz</t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : Level</t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : Durchschnittliche Bearbeitungszeit, Format ist unter http://www.w3.org/TR/xmlschema-2/#duration definiert</t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : Itemschwierigkeit (zwischen 0.0 und 1.0)</t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : Standardabweichung Itemschwierigkeit (zwischen 0.0 und 1.0)</t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : Trennschärfe (zwischen -1.0 und 1.0)</t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : Anzahl Distraktoren ( 1 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional, nur in Fragenpool : Editor </t>
+  </si>
+  <si>
+    <t>Optional, nur in Fragenpool : Editor Version</t>
+  </si>
+  <si>
+    <t>Fragetpy: Fill in the blanks (Lückentext)</t>
   </si>
 </sst>
 </file>
@@ -363,9 +363,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -395,18 +399,22 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="16">
     <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Erklärender Text" xfId="1" builtinId="53"/>
     <cellStyle name="Link" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -739,7 +747,7 @@
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="A1:C22"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -753,16 +761,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -770,194 +778,194 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30">
+      <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="B10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1">
         <v>0.55000000000000004</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1">
         <v>0.6</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1">
         <v>-0.33</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="D20" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -965,18 +973,18 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45">
       <c r="D22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -984,7 +992,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>1</v>
@@ -993,22 +1001,22 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B27" s="1">
         <v>5</v>
@@ -1017,10 +1025,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" s="4"/>
     </row>
@@ -1029,19 +1037,19 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" s="4"/>
     </row>
@@ -1050,16 +1058,16 @@
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" s="4"/>
     </row>
@@ -1068,16 +1076,16 @@
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="4"/>
     </row>
@@ -1092,54 +1100,54 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30">
       <c r="A39" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="45">
       <c r="A40" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B41" s="1">
         <v>3</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1147,10 +1155,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1158,10 +1166,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1169,10 +1177,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1180,10 +1188,10 @@
         <v>-1</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1191,10 +1199,10 @@
         <v>-1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1202,10 +1210,10 @@
         <v>-1</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1213,15 +1221,15 @@
         <v>-1</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30">
       <c r="D49" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1235,54 +1243,54 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="30">
       <c r="A54" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="30">
       <c r="A55" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B56" s="1">
         <v>1</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1290,10 +1298,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1301,10 +1309,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1312,10 +1320,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1323,10 +1331,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1334,10 +1342,10 @@
         <v>1</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1345,10 +1353,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1356,15 +1364,15 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="30">
       <c r="D64" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OO-1209 adding context help for import EN, improve import button in editor
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti/questionimport/qti-import-metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31240" windowHeight="28280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43280" windowHeight="28280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
   <si>
     <t>Typ</t>
   </si>
@@ -48,15 +48,9 @@
     <t>Ein Text element</t>
   </si>
   <si>
-    <t>verbannen</t>
-  </si>
-  <si>
     <t>20,50</t>
   </si>
   <si>
-    <t>Eine Lücke, Länge 20, Anzahl Zeichen 50. Wenn richtig gibt’s einen Punkt</t>
-  </si>
-  <si>
     <t>Es können beliebig viele Text und Lückenelemente aufgelistet werden. Die Leerzeile markiert das Ende des Frageitems. Die nächste Zeile sollte wieder mit „Typ“ beginnen und markiert den Beginn des nächsten Frageitems.</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>Im Jahr 1982 wurde die WM in Spanien ausgetragen.</t>
   </si>
   <si>
-    <t>Welche Mannschaft gewann 1982 die Fussball Weltmeisterschaft=</t>
-  </si>
-  <si>
     <t>Spanien</t>
   </si>
   <si>
@@ -292,13 +283,25 @@
   </si>
   <si>
     <t>Fragetpy: Fill in the blanks (Lückentext)</t>
+  </si>
+  <si>
+    <t>Welche Mannschaft gewann 1982 die Fussball Weltmeisterschaft?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zweites Lücktentextbeispiel mit mehreren zum Teil leeren Lücken. </t>
+  </si>
+  <si>
+    <t>verbannen;Verbot</t>
+  </si>
+  <si>
+    <t>Eine Lücke, Länge 20, Anzahl Zeichen 50. Wenn richtig gibt’s einen Punkt. Strickpunkt trennt Synonyme bzw. mehrere korrekte Lösungen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -345,16 +348,56 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -362,8 +405,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -380,8 +438,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -395,11 +472,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="16" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="16" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="16" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="16" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="16" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="35">
+    <cellStyle name="Ausgabe" xfId="16" builtinId="21"/>
     <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="7" builtinId="9" hidden="1"/>
@@ -407,6 +506,15 @@
     <cellStyle name="Besuchter Link" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Erklärender Text" xfId="1" builtinId="53"/>
     <cellStyle name="Link" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
@@ -415,6 +523,15 @@
     <cellStyle name="Link" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -746,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -761,389 +878,428 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>90</v>
+      <c r="C3" s="7"/>
+      <c r="D3" s="12" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="7"/>
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
-      <c r="A5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="A5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="7"/>
       <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30">
+      <c r="A10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+    <row r="12" spans="1:4" ht="30">
+      <c r="A12" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30">
-      <c r="A10" s="1" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B13" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="8">
+        <v>-0.33</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30">
-      <c r="A12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="1">
-        <v>-0.33</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C18" s="7"/>
+      <c r="D18" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="1">
+    <row r="19" spans="1:4">
+      <c r="A19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="7">
         <v>1</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
+      <c r="C19" s="7"/>
       <c r="D19" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C20" s="7"/>
       <c r="D20" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1">
+    <row r="21" spans="1:4" ht="30">
+      <c r="A21" s="5">
         <v>1</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="4" t="s">
+    </row>
+    <row r="23" spans="1:4">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="45">
-      <c r="D22" s="4" t="s">
+      <c r="C25" s="7"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="7">
+        <v>5</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="C28" s="7"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="5">
         <v>1</v>
       </c>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="B29" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="1">
-        <v>5</v>
-      </c>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1" t="s">
+      <c r="C29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B30" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="5">
+        <v>1</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1">
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="5">
         <v>1</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B34" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="C34" s="7"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="B35" s="10"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="B36" s="10"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="45">
+      <c r="A40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="45">
-      <c r="A40" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="1">
+      <c r="B41" s="7">
         <v>3</v>
       </c>
       <c r="D41" s="4" t="s">
@@ -1151,142 +1307,145 @@
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="1">
+      <c r="A42" s="5">
         <v>1</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="5">
+        <v>1</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D43" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="5">
+        <v>1</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="1">
-        <v>1</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="D44" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1">
-        <v>1</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="D45" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1">
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="5">
         <v>-1</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D46" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1">
+      <c r="D47" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="5">
         <v>-1</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B48" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="1">
-        <v>-1</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="D48" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="30">
+      <c r="B49" s="10"/>
+      <c r="D49" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="1">
-        <v>-1</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="30">
-      <c r="D49" s="4" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="50" spans="1:4">
+      <c r="B50" s="10"/>
       <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4">
+      <c r="B51" s="10"/>
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="30">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="30">
+      <c r="A55" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="30">
-      <c r="A55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B56" s="1">
+      <c r="B56" s="7">
         <v>1</v>
       </c>
       <c r="D56" s="4" t="s">
@@ -1294,85 +1453,85 @@
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="1">
+      <c r="A57" s="5">
         <v>0</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="5">
+        <v>0</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D57" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="1">
+      <c r="D58" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="5">
         <v>0</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="1">
+      <c r="B59" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="5">
         <v>0</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="1">
+      <c r="B60" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="5">
+        <v>1</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="5">
         <v>0</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B62" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D60" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="1">
-        <v>1</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="1">
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="5">
         <v>0</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="1">
-        <v>0</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>33</v>
+      <c r="B63" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="30">
       <c r="D64" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OO-1551: add fields for feedback on correct and wrong answers
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti/questionimport/qti-import-metadata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43280" windowHeight="28280" tabRatio="500"/>
+    <workbookView xWindow="8400" yWindow="0" windowWidth="30700" windowHeight="27140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="97">
   <si>
     <t>Typ</t>
   </si>
@@ -295,6 +295,21 @@
   </si>
   <si>
     <t>Eine Lücke, Länge 20, Anzahl Zeichen 50. Wenn richtig gibt’s einen Punkt. Strickpunkt trennt Synonyme bzw. mehrere korrekte Lösungen</t>
+  </si>
+  <si>
+    <t>Feedback correct answer</t>
+  </si>
+  <si>
+    <t>Feedback wrong answer</t>
+  </si>
+  <si>
+    <t>Bravo! Die Antwort ich absolut korrekt weil ban wirklich verbannen heisst.</t>
+  </si>
+  <si>
+    <t>Leider falsch. Probieren Sie es noch einmal. Tip: das Englische Wort ist sehr ähnlich wie das deutsch Wort!</t>
+  </si>
+  <si>
+    <t>Optional</t>
   </si>
 </sst>
 </file>
@@ -421,7 +436,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -439,6 +454,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -497,7 +516,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="39">
     <cellStyle name="Ausgabe" xfId="16" builtinId="21"/>
     <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
@@ -515,6 +534,8 @@
     <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Erklärender Text" xfId="1" builtinId="53"/>
     <cellStyle name="Link" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
@@ -532,6 +553,8 @@
     <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -861,15 +884,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:B56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
     <col min="4" max="4" width="91.33203125" style="2" customWidth="1"/>
@@ -1069,128 +1092,130 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="30">
       <c r="A18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>73</v>
+        <v>92</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="7">
-        <v>1</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45">
+      <c r="A19" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="4" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>7</v>
+      <c r="A20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30">
-      <c r="A21" s="5">
+    <row r="23" spans="1:4" ht="30">
+      <c r="A23" s="5">
         <v>1</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="4" t="s">
+    <row r="24" spans="1:4" ht="45">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:4">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B26" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="4" t="s">
+      <c r="C26" s="7"/>
+      <c r="D26" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="7">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="A28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="8"/>
       <c r="C28" s="7"/>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="5">
-        <v>1</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="A29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="7">
+        <v>5</v>
+      </c>
+      <c r="C29" s="7"/>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4">
@@ -1198,7 +1223,7 @@
         <v>6</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="4"/>
@@ -1207,7 +1232,9 @@
       <c r="A31" s="5">
         <v>1</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="C31" s="7" t="s">
         <v>14</v>
       </c>
@@ -1218,7 +1245,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="4"/>
@@ -1238,94 +1265,92 @@
         <v>6</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="B35" s="10"/>
+      <c r="A35" s="5">
+        <v>1</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="B36" s="10"/>
+      <c r="A36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="7"/>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="5" t="s">
+      <c r="B37" s="10"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="B38" s="10"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B39" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D39" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="5" t="s">
+    <row r="40" spans="1:4">
+      <c r="A40" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B40" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30">
-      <c r="A39" s="6" t="s">
+    <row r="41" spans="1:4" ht="30">
+      <c r="A41" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B41" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D41" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="45">
-      <c r="A40" s="5" t="s">
+    <row r="42" spans="1:4" ht="45">
+      <c r="A42" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B42" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="5" t="s">
+    <row r="43" spans="1:4">
+      <c r="A43" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B43" s="7">
         <v>3</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="5">
-        <v>1</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="5">
-        <v>1</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1333,7 +1358,7 @@
         <v>1</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>24</v>
@@ -1341,24 +1366,24 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1366,7 +1391,7 @@
         <v>-1</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>28</v>
@@ -1377,101 +1402,101 @@
         <v>-1</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30">
-      <c r="B49" s="10"/>
+    <row r="49" spans="1:4">
+      <c r="A49" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="D49" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="30">
+      <c r="B51" s="10"/>
+      <c r="D51" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="B50" s="10"/>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="B51" s="10"/>
-      <c r="D51" s="4"/>
-    </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="5" t="s">
+      <c r="B52" s="10"/>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="B53" s="10"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B54" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D54" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="5" t="s">
+    <row r="55" spans="1:4">
+      <c r="A55" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B55" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D55" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30">
-      <c r="A54" s="6" t="s">
+    <row r="56" spans="1:4" ht="30">
+      <c r="A56" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B56" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D56" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="30">
-      <c r="A55" s="5" t="s">
+    <row r="57" spans="1:4" ht="30">
+      <c r="A57" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B57" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D57" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="5" t="s">
+    <row r="58" spans="1:4">
+      <c r="A58" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B58" s="7">
         <v>1</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D58" s="4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="5">
-        <v>0</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="5">
-        <v>0</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1479,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>46</v>
@@ -1490,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>46</v>
@@ -1498,13 +1523,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1512,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>46</v>
@@ -1520,17 +1545,39 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="5">
+        <v>1</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="5">
         <v>0</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B64" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="5">
+        <v>0</v>
+      </c>
+      <c r="B65" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D65" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="30">
-      <c r="D64" s="4" t="s">
+    <row r="66" spans="1:4" ht="30">
+      <c r="D66" s="4" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>